<commit_message>
Code update 1.3.25 , 3.33 PM
</commit_message>
<xml_diff>
--- a/uploads/brt_master.xlsx
+++ b/uploads/brt_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1727AEC7-395D-429B-A5A8-2BF6AA4C6330}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BB0D6D-0EBA-4006-B503-148D08D63626}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>brt_id</t>
   </si>
@@ -46,25 +46,49 @@
     <t>brt_corridor_km</t>
   </si>
   <si>
+    <t>B 1</t>
+  </si>
+  <si>
     <t>संगमवाडी - विश्रांतवाडी (१)</t>
   </si>
   <si>
+    <t>B 2</t>
+  </si>
+  <si>
     <t>सांगवी- किवळे मुकाई चौक (२)</t>
   </si>
   <si>
+    <t>B 3</t>
+  </si>
+  <si>
     <t>नाशिक फाटा - वाकड चौक (३)</t>
   </si>
   <si>
+    <t>B 4</t>
+  </si>
+  <si>
     <t>येरवडा - आपले घर (४)</t>
   </si>
   <si>
+    <t>B 5</t>
+  </si>
+  <si>
     <t>निगडी - दापोडी (५)</t>
   </si>
   <si>
+    <t>B 6</t>
+  </si>
+  <si>
     <t>कात्रज - स्‍वारगेट (६)</t>
   </si>
   <si>
+    <t>B 7</t>
+  </si>
+  <si>
     <t>चिखली - काळेवाडी फाटा (७)</t>
+  </si>
+  <si>
+    <t>B 8</t>
   </si>
   <si>
     <t>दिघी - आळंदी (८)</t>
@@ -102,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -110,29 +134,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,254 +453,234 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="42.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
         <v>972</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>99</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>81</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1099</v>
+      </c>
+      <c r="E3" s="3">
+        <v>120</v>
+      </c>
+      <c r="F3" s="3">
+        <v>112</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>198</v>
+      </c>
+      <c r="E4" s="3">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1785</v>
+      </c>
+      <c r="E5" s="3">
+        <v>179</v>
+      </c>
+      <c r="F5" s="3">
+        <v>162</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
-        <v>21167.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1099</v>
-      </c>
-      <c r="E3">
-        <v>120</v>
-      </c>
-      <c r="F3">
-        <v>112</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3">
-        <v>28322.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>198</v>
-      </c>
-      <c r="E4">
+      <c r="D6" s="3">
+        <v>1986</v>
+      </c>
+      <c r="E6" s="3">
+        <v>202</v>
+      </c>
+      <c r="F6" s="3">
+        <v>164</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2053</v>
+      </c>
+      <c r="E7" s="3">
+        <v>181</v>
+      </c>
+      <c r="F7" s="3">
+        <v>155</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4">
-        <v>4667.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1785</v>
-      </c>
-      <c r="E5">
-        <v>179</v>
-      </c>
-      <c r="F5">
-        <v>162</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5">
-        <v>41478.699999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>1986</v>
-      </c>
-      <c r="E6">
-        <v>202</v>
-      </c>
-      <c r="F6">
-        <v>164</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6">
-        <v>46960.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>2053</v>
-      </c>
-      <c r="E7">
-        <v>181</v>
-      </c>
-      <c r="F7">
-        <v>155</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7">
-        <v>34533.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>444</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>41</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>32</v>
       </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8">
-        <v>8945.1</v>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
         <v>631</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>60</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>46</v>
       </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9">
-        <v>13860.2</v>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>